<commit_message>
leave gpio12 floating, add diode
</commit_message>
<xml_diff>
--- a/hardware/rev_a/embedded-gw_bom.xlsx
+++ b/hardware/rev_a/embedded-gw_bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="149">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -49,13 +49,16 @@
     <t xml:space="preserve">MPN</t>
   </si>
   <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
     <t xml:space="preserve">DIODE_ZENER0201</t>
   </si>
   <si>
     <t xml:space="preserve">0201_DIODE</t>
   </si>
   <si>
-    <t xml:space="preserve">D1</t>
+    <t xml:space="preserve">D1,D2</t>
   </si>
   <si>
     <t xml:space="preserve">ESD7381MUT5GOSCT-ND</t>
@@ -118,7 +121,7 @@
     <t xml:space="preserve">10k</t>
   </si>
   <si>
-    <t xml:space="preserve">R10,R11,R12,R13</t>
+    <t xml:space="preserve">R10,R11,R12,R13,R15,R16</t>
   </si>
   <si>
     <t xml:space="preserve">RMCF0402JT10K0CT-ND</t>
@@ -157,6 +160,18 @@
     <t xml:space="preserve">GCM1555C1H120GA16D</t>
   </si>
   <si>
+    <t xml:space="preserve">1k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R17,R18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF0402JT1K00CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMCF0402JT1K00</t>
+  </si>
+  <si>
     <t xml:space="preserve">4.7uF</t>
   </si>
   <si>
@@ -223,6 +238,21 @@
     <t xml:space="preserve">AP7362A-33SP-13 </t>
   </si>
   <si>
+    <t xml:space="preserve">B3U-1000P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1,S2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW1020CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omron</t>
+  </si>
+  <si>
     <t xml:space="preserve">BLUE</t>
   </si>
   <si>
@@ -232,7 +262,7 @@
     <t xml:space="preserve">LED-0603</t>
   </si>
   <si>
-    <t xml:space="preserve">D7,D8,D11</t>
+    <t xml:space="preserve">D8,D9,D12</t>
   </si>
   <si>
     <t xml:space="preserve">LED</t>
@@ -301,13 +331,31 @@
     <t xml:space="preserve">Hirose Connector</t>
   </si>
   <si>
+    <t xml:space="preserve">DMN32D2LDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT353</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common source dual n-channel mosfet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DMN32D2LDF-7DICT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DMN32D2LDF-7</t>
+  </si>
+  <si>
     <t xml:space="preserve">EMIF06-MSD01F2</t>
   </si>
   <si>
     <t xml:space="preserve">BGA16C50P4X4_192X192X65N</t>
   </si>
   <si>
-    <t xml:space="preserve">D2</t>
+    <t xml:space="preserve">D3</t>
   </si>
   <si>
     <t xml:space="preserve">Mini and micro SD Card - EMI filtering and 25 kV ESD protection</t>
@@ -352,7 +400,7 @@
     <t xml:space="preserve">JS202011CQN</t>
   </si>
   <si>
-    <t xml:space="preserve">S2</t>
+    <t xml:space="preserve">S3</t>
   </si>
   <si>
     <t xml:space="preserve">DPDT through hole</t>
@@ -367,7 +415,7 @@
     <t xml:space="preserve">RED</t>
   </si>
   <si>
-    <t xml:space="preserve">D3,D5,D9</t>
+    <t xml:space="preserve">D4,D6,D10</t>
   </si>
   <si>
     <t xml:space="preserve">160-1830-1-ND</t>
@@ -412,7 +460,7 @@
     <t xml:space="preserve">YELLOW</t>
   </si>
   <si>
-    <t xml:space="preserve">D4,D6,D10</t>
+    <t xml:space="preserve">D5,D7,D11</t>
   </si>
   <si>
     <t xml:space="preserve">160-1831-1-ND</t>
@@ -514,10 +562,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -525,7 +573,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="98.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.68"/>
@@ -560,25 +608,28 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,25 +637,25 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,25 +663,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -641,48 +692,48 @@
         <v>100</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -690,25 +741,25 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -716,106 +767,103 @@
         <v>2</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="D9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="F9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="0" t="s">
+      <c r="I9" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>470</v>
+        <v>1</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>50</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>54</v>
+        <v>6</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>470</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>56</v>
       </c>
       <c r="F11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="I11" s="0" t="s">
         <v>58</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,112 +871,112 @@
         <v>1</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="0" t="s">
+      <c r="E12" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="F12" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="G12" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="H12" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="I12" s="0" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="F13" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="G13" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="H13" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="I13" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="0" t="s">
+      <c r="G14" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="H14" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="I14" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" s="0" t="s">
+      <c r="F15" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="G15" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="I15" s="0" t="s">
         <v>83</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -936,28 +984,28 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="0" t="s">
+      <c r="G16" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="H16" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>92</v>
-      </c>
       <c r="I16" s="0" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,28 +1013,28 @@
         <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="D17" s="0" t="s">
+      <c r="G17" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="H17" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="I17" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -994,33 +1042,39 @@
         <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="D18" s="0" t="s">
+      <c r="F18" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="G18" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="H18" s="0" t="s">
         <v>102</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>104</v>
@@ -1028,11 +1082,14 @@
       <c r="E19" s="0" t="s">
         <v>105</v>
       </c>
+      <c r="F19" s="0" t="s">
+        <v>106</v>
+      </c>
       <c r="G19" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>107</v>
+        <v>70</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>108</v>
@@ -1049,19 +1106,19 @@
         <v>109</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I20" s="0" t="s">
         <v>109</v>
@@ -1069,48 +1126,51 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>68</v>
+        <v>115</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>71</v>
+        <v>117</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="J22" s="0" t="s">
         <v>121</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,28 +1178,28 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F23" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="I23" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1147,25 +1207,100 @@
         <v>3</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>